<commit_message>
release: prepare npnameyrapp v1.1 (scripts, data, docs, images, .Rprofile)
</commit_message>
<xml_diff>
--- a/data/ctTable/CT_TABLE.xlsx
+++ b/data/ctTable/CT_TABLE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\wildlife\previous\baluran\cameraTrap\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\NEU\evolveApp0\npnameyrapp-master\data\ctTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C8E6BD-5945-4D38-B02C-49EFF5EA7487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AA7F88-E2DA-4CA1-9B43-78B4A4F406B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="speciesevents" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Station_ID</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>CTC</t>
+  </si>
+  <si>
+    <t>CTD</t>
   </si>
 </sst>
 </file>
@@ -51,7 +54,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -84,7 +87,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -479,6 +482,23 @@
         <v>42278</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>9134567</v>
+      </c>
+      <c r="C5">
+        <v>213394</v>
+      </c>
+      <c r="D5" s="1">
+        <v>42277</v>
+      </c>
+      <c r="E5" s="1">
+        <v>42278</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>